<commit_message>
Update Interactive Resume Data.xlsx
</commit_message>
<xml_diff>
--- a/Interactive Resume/Interactive Resume Data.xlsx
+++ b/Interactive Resume/Interactive Resume Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.reynolds\Github_MachineLearning\Visualizations\Interactive Resume\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamr\Documents\GitHub\Visualizations\Interactive Resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AB19DD5-314B-4CA3-8E1C-7B10EA9E52CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8EEBC-698D-4D4E-86F5-F66DD9A48B20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2565" windowWidth="22050" windowHeight="18210" xr2:uid="{36519C5B-B072-4700-8336-CF78A2B489E9}"/>
+    <workbookView xWindow="5745" yWindow="960" windowWidth="21600" windowHeight="12780" activeTab="1" xr2:uid="{36519C5B-B072-4700-8336-CF78A2B489E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
-    <sheet name="notes" sheetId="3" r:id="rId2"/>
-    <sheet name="Skills" sheetId="2" r:id="rId3"/>
+    <sheet name="Skills" sheetId="2" r:id="rId2"/>
+    <sheet name="notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>category</t>
   </si>
@@ -54,6 +53,152 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>Southern Utah University</t>
+  </si>
+  <si>
+    <t>Boston University</t>
+  </si>
+  <si>
+    <t>M.S. Computer information Systems</t>
+  </si>
+  <si>
+    <t>B.S. Mathematics</t>
+  </si>
+  <si>
+    <t>Cedar City, UT</t>
+  </si>
+  <si>
+    <t>Boston, MA</t>
+  </si>
+  <si>
+    <t>Utah Local Governments Trust</t>
+  </si>
+  <si>
+    <t>Western Governors University</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Junior Jazz Basketball</t>
+  </si>
+  <si>
+    <t>Wyzant Tutoring</t>
+  </si>
+  <si>
+    <t>Research Analyst</t>
+  </si>
+  <si>
+    <t>Math Tutor</t>
+  </si>
+  <si>
+    <t>Salt Lake City, UT</t>
+  </si>
+  <si>
+    <t>North Salt Lake City, UT</t>
+  </si>
+  <si>
+    <t>Data Analyst / Underwriter</t>
+  </si>
+  <si>
+    <t>Recreational</t>
+  </si>
+  <si>
+    <t>Pickleball</t>
+  </si>
+  <si>
+    <t>Volleyball</t>
+  </si>
+  <si>
+    <t>Coach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• </t>
+  </si>
+  <si>
+    <t>• Emphasis: Actuarial Science
+• Summa Cum Laude
+• 3.9 GPA</t>
+  </si>
+  <si>
+    <t>• Subconcentration: Data Analytics
+• 
+• 3.6 GPA</t>
+  </si>
+  <si>
+    <t>• Created underwriting pricing model using machine learning
+• Analyzed and identified loss trends for property, workers compensation, and automobile insurance lines</t>
+  </si>
+  <si>
+    <t>• Develop forecasts using time series and machine learning methods to predict future outcomes
+• Create and distribute executive level dashboards and reports using Tableau and Cognos
+• Work with data throughout the ETL process with APIs, SQL object creation and job scheduling
+• Perform ad-hoc analysis to support university initiatives</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Apache Spark</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Tableau</t>
+  </si>
+  <si>
+    <t>IBM Cognos</t>
+  </si>
+  <si>
+    <t>Regression Analysis</t>
+  </si>
+  <si>
+    <t>Decision Trees/ Random Forest</t>
+  </si>
+  <si>
+    <t>Time Series Analysis</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>years_experience</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>• Play beach and indoor volleyball in the Beehive Social League</t>
+  </si>
+  <si>
+    <t>• Coached a Jr. Jazz team of 2nd and 3rd graders in Salt Lake City</t>
+  </si>
+  <si>
+    <t>• Tutored high school and college math students in statistics, algegra, and calculus</t>
+  </si>
+  <si>
+    <t>• Play pickleball with friends and played in 2 tournaments although the results of these tournaments will not be disclosed</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -97,9 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,17 +700,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A11812B-D75E-49B2-BC46-E29CFA7297D0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -585,6 +737,217 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40770</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42125</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42740</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43490</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>42156</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43021</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43024</v>
+      </c>
+      <c r="D5" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43716</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42217</v>
+      </c>
+      <c r="D6" s="2">
+        <v>42767</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43497</v>
+      </c>
+      <c r="D7" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43716</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
+        <v>42309</v>
+      </c>
+      <c r="D8" s="2">
+        <v>42401</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43586</v>
+      </c>
+      <c r="D9" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43716</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43282</v>
+      </c>
+      <c r="D10" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43716</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -594,10 +957,181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6161E2B4-894F-49EC-A060-9B1F12E0D676}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38419D3-0D4B-47E6-87A9-C10EA1D4C6F5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -606,16 +1140,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6161E2B4-894F-49EC-A060-9B1F12E0D676}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>